<commit_message>
Changes to WEB API
</commit_message>
<xml_diff>
--- a/Jquery/JQuery Notes.xlsx
+++ b/Jquery/JQuery Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jquery" sheetId="1" r:id="rId1"/>
@@ -2605,9 +2605,6 @@
     </r>
   </si>
   <si>
-    <t>Resturns value of checkbox checked (VALUE='value') of HTML</t>
-  </si>
-  <si>
     <r>
       <t>$(</t>
     </r>
@@ -3890,6 +3887,9 @@
       </rPr>
       <t> (request, status, error) {</t>
     </r>
+  </si>
+  <si>
+    <t>Returns value of checkbox checked (VALUE='value') of HTML</t>
   </si>
 </sst>
 </file>
@@ -4436,8 +4436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4759,26 +4759,26 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B54" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B55" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B56" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -5031,40 +5031,40 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5077,8 +5077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5108,23 +5108,23 @@
         <v>192</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" t="s">
         <v>194</v>
-      </c>
-      <c r="B9" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" t="s">
         <v>196</v>
-      </c>
-      <c r="B11" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -5387,10 +5387,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -5441,7 +5441,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -5475,260 +5475,260 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>309</v>
+      </c>
+      <c r="B37" t="s">
         <v>310</v>
-      </c>
-      <c r="B37" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>311</v>
+      </c>
+      <c r="B38" t="s">
         <v>312</v>
-      </c>
-      <c r="B38" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C40" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B41" t="s">
         <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B46" t="s">
         <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" s="18" t="s">
         <v>317</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>318</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>319</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -5753,38 +5753,38 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
         <v>242</v>
-      </c>
-      <c r="B2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B4" t="s">
         <v>245</v>
-      </c>
-      <c r="B4" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5792,17 +5792,17 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5810,17 +5810,17 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5828,17 +5828,17 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5846,22 +5846,22 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -5869,22 +5869,22 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -5892,7 +5892,7 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -5900,7 +5900,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -5908,7 +5908,7 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -5935,81 +5935,81 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>266</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" t="s">
         <v>268</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>269</v>
       </c>
-      <c r="C3" t="s">
-        <v>270</v>
-      </c>
       <c r="D3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" t="s">
         <v>268</v>
       </c>
-      <c r="B4" t="s">
-        <v>269</v>
-      </c>
       <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" t="s">
         <v>274</v>
-      </c>
-      <c r="D4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" t="s">
         <v>276</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5" t="s">
         <v>277</v>
-      </c>
-      <c r="C5" t="s">
-        <v>274</v>
-      </c>
-      <c r="D5" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -6033,10 +6033,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6046,39 +6046,39 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -6086,7 +6086,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>